<commit_message>
Update WarriorHub Effort Estimation.xlsx
</commit_message>
<xml_diff>
--- a/WarriorHub Effort Estimation.xlsx
+++ b/WarriorHub Effort Estimation.xlsx
@@ -2070,7 +2070,13 @@
         <v>81</v>
       </c>
       <c r="C60" s="3">
-        <v>3.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="D60" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E60" s="3">
+        <v>1.0</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>9</v>

</xml_diff>